<commit_message>
Minor graph title change
</commit_message>
<xml_diff>
--- a/Results/data_bench_test.xlsx
+++ b/Results/data_bench_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucapaccard/Documents/INSA/4A/S8/Capteurs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7BD2FC52-7D34-DB4A-979D-43BD0A65E904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C91350-1B53-CA43-984C-F221C0E55F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{E90387A7-1533-4F47-B14B-28CE7B200960}"/>
   </bookViews>
@@ -1872,7 +1872,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> 2H tension</a:t>
+              <a:t> 2H compression</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -2522,7 +2522,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Pencil 2B tension</a:t>
+              <a:t>Pencil 2B compression</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3171,7 +3171,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>Pencil HB tension</a:t>
+              <a:t>Pencil HB compression</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -12923,8 +12923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B6F0A65-5F7C-AC40-B216-07E9FC2FA631}">
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="U38" sqref="U38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14237,8 +14237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A9BAF04-6FC7-CE48-AE14-9D2C2252560B}">
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="Q40" sqref="Q40"/>
+    <sheetView showGridLines="0" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A77" sqref="A62:J77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update nbre de chiffres significatifs
</commit_message>
<xml_diff>
--- a/Results/data_bench_test.xlsx
+++ b/Results/data_bench_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucapaccard/Documents/INSA/4A/S8/Capteurs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C91350-1B53-CA43-984C-F221C0E55F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAB62CC-4651-4B42-8811-FCC09A15D3D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{E90387A7-1533-4F47-B14B-28CE7B200960}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{E90387A7-1533-4F47-B14B-28CE7B200960}"/>
   </bookViews>
   <sheets>
     <sheet name="Compression" sheetId="2" r:id="rId1"/>
@@ -110,6 +110,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -340,7 +343,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -790,11 +793,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -805,10 +821,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
@@ -879,25 +893,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="22" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="25" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -916,66 +920,22 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="29" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -994,30 +954,6 @@
     <xf numFmtId="0" fontId="2" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="27" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1027,25 +963,123 @@
     <xf numFmtId="0" fontId="2" fillId="27" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="17" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="17" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="17" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="20" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="20" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="20" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="23" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="23" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="23" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="11" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="26" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="26" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="5" fillId="26" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="17" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="17" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="20" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="20" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="23" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="23" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="26" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="26" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1190,7 +1224,7 @@
             <c:numRef>
               <c:f>Compression!$A$6:$A$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1223,7 +1257,7 @@
             <c:numRef>
               <c:f>Compression!$N$6:$N$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1306,7 +1340,7 @@
             <c:numRef>
               <c:f>Compression!$A$28:$A$35</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1339,7 +1373,7 @@
             <c:numRef>
               <c:f>Compression!$N$28:$N$35</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1422,7 +1456,7 @@
             <c:numRef>
               <c:f>Compression!$A$17:$A$24</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1455,7 +1489,7 @@
             <c:numRef>
               <c:f>Compression!$N$17:$N$24</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1583,7 +1617,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1709,7 +1743,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1960,7 +1994,7 @@
             <c:numRef>
               <c:f>Compression!$A$17:$A$24</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -1993,7 +2027,7 @@
             <c:numRef>
               <c:f>Compression!$B$17:$B$24</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -2076,7 +2110,7 @@
             <c:numRef>
               <c:f>Compression!$G$17:$G$24</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -2109,7 +2143,7 @@
             <c:numRef>
               <c:f>Compression!$H$17:$H$24</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -2237,7 +2271,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2363,7 +2397,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2609,7 +2643,7 @@
             <c:numRef>
               <c:f>Compression!$A$6:$A$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -2642,7 +2676,7 @@
             <c:numRef>
               <c:f>Compression!$B$6:$B$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -2725,7 +2759,7 @@
             <c:numRef>
               <c:f>Compression!$G$6:$G$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -2758,7 +2792,7 @@
             <c:numRef>
               <c:f>Compression!$H$6:$H$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -2886,7 +2920,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3012,7 +3046,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3258,7 +3292,7 @@
             <c:numRef>
               <c:f>Compression!$A$28:$A$35</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -3291,7 +3325,7 @@
             <c:numRef>
               <c:f>Compression!$B$28:$B$35</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -3374,7 +3408,7 @@
             <c:numRef>
               <c:f>Compression!$G$28:$G$35</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -3407,7 +3441,7 @@
             <c:numRef>
               <c:f>Compression!$H$28:$H$35</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -3535,7 +3569,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3657,7 +3691,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3918,7 +3952,7 @@
             <c:numRef>
               <c:f>Tension!$A$6:$A$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -3951,7 +3985,7 @@
             <c:numRef>
               <c:f>Tension!$N$6:$N$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -4034,7 +4068,7 @@
             <c:numRef>
               <c:f>Tension!$M$28:$M$35</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -4067,7 +4101,7 @@
             <c:numRef>
               <c:f>Tension!$N$28:$N$35</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -4150,7 +4184,7 @@
             <c:numRef>
               <c:f>Tension!$A$39:$A$46</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -4183,7 +4217,7 @@
             <c:numRef>
               <c:f>Tension!$N$39:$N$46</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -4266,7 +4300,7 @@
             <c:numRef>
               <c:f>Tension!$A$17:$A$24</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -4299,7 +4333,7 @@
             <c:numRef>
               <c:f>Tension!$N$17:$N$24</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -4427,7 +4461,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4553,7 +4587,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4804,7 +4838,7 @@
             <c:numRef>
               <c:f>Tension!$A$17:$A$24</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -4837,7 +4871,7 @@
             <c:numRef>
               <c:f>Tension!$B$17:$B$24</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -4920,7 +4954,7 @@
             <c:numRef>
               <c:f>Tension!$G$17:$G$24</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -4953,7 +4987,7 @@
             <c:numRef>
               <c:f>Tension!$H$17:$H$24</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -5081,7 +5115,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5207,7 +5241,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5453,7 +5487,7 @@
             <c:numRef>
               <c:f>Tension!$A$6:$A$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -5486,7 +5520,7 @@
             <c:numRef>
               <c:f>Tension!$B$6:$B$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -5569,7 +5603,7 @@
             <c:numRef>
               <c:f>Tension!$G$6:$G$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -5602,7 +5636,7 @@
             <c:numRef>
               <c:f>Tension!$H$6:$H$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -5730,7 +5764,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5856,7 +5890,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6102,7 +6136,7 @@
             <c:numRef>
               <c:f>Tension!$A$39:$A$46</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -6135,7 +6169,7 @@
             <c:numRef>
               <c:f>Tension!$B$39:$B$46</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -6218,7 +6252,7 @@
             <c:numRef>
               <c:f>Tension!$G$39:$G$46</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -6251,7 +6285,7 @@
             <c:numRef>
               <c:f>Tension!$H$39:$H$46</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -6379,7 +6413,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6501,7 +6535,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6747,7 +6781,7 @@
             <c:numRef>
               <c:f>Tension!$A$28:$A$35</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -6780,7 +6814,7 @@
             <c:numRef>
               <c:f>Tension!$B$28:$B$35</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -6863,7 +6897,7 @@
             <c:numRef>
               <c:f>Tension!$G$28:$G$35</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -6896,7 +6930,7 @@
             <c:numRef>
               <c:f>Tension!$H$28:$H$35</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -7028,7 +7062,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -7154,7 +7188,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -12287,15 +12321,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>825500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12324,16 +12358,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>768350</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>44450</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12362,16 +12396,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>298450</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>196850</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>107950</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12400,16 +12434,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12443,16 +12477,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>850900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12479,16 +12513,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>895350</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12515,16 +12549,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>692150</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>793750</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12551,16 +12585,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>755650</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12587,16 +12621,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>222250</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>615950</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>463550</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12921,10 +12955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B6F0A65-5F7C-AC40-B216-07E9FC2FA631}">
-  <dimension ref="A1:Q35"/>
+  <dimension ref="A1:AA35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="U38" sqref="U38"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12948,129 +12982,129 @@
     <col min="18" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="113" t="s">
+    <row r="1" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="115"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="79"/>
     </row>
-    <row r="2" spans="1:17" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="P2" s="41" t="s">
+    <row r="2" spans="1:27" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="Z2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="100" t="s">
+      <c r="AA2" s="67" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="116" t="s">
+    <row r="3" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="117"/>
-      <c r="C3" s="117"/>
-      <c r="D3" s="117"/>
-      <c r="E3" s="118"/>
-      <c r="G3" s="127" t="s">
+      <c r="B3" s="81"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="82"/>
+      <c r="G3" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="128"/>
-      <c r="I3" s="128"/>
-      <c r="J3" s="128"/>
-      <c r="K3" s="129"/>
-      <c r="M3" s="127" t="s">
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="85"/>
+      <c r="M3" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="129"/>
-      <c r="P3" s="46">
+      <c r="N3" s="85"/>
+      <c r="Z3" s="44">
         <v>0</v>
       </c>
-      <c r="Q3" s="42" t="s">
+      <c r="AA3" s="40" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="101" t="s">
+    <row r="4" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="102"/>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="103"/>
-      <c r="G4" s="130" t="s">
+      <c r="B4" s="87"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="87"/>
+      <c r="E4" s="88"/>
+      <c r="G4" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="131"/>
-      <c r="M4" s="119" t="s">
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="87"/>
+      <c r="K4" s="90"/>
+      <c r="M4" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="120"/>
-      <c r="P4" s="47">
+      <c r="N4" s="92"/>
+      <c r="Z4" s="45">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="Q4" s="43">
+      <c r="AA4" s="41">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:27" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="59" t="s">
+      <c r="G5" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="60" t="s">
+      <c r="K5" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="49" t="s">
+      <c r="M5" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="N5" s="69" t="s">
+      <c r="N5" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="47">
+      <c r="Z5" s="45">
         <v>3.333333E-3</v>
       </c>
-      <c r="Q5" s="44">
+      <c r="AA5" s="42">
         <v>4.5</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A6" s="110">
         <v>0</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="108">
         <v>0</v>
       </c>
       <c r="C6" s="3">
@@ -13083,10 +13117,10 @@
         <f>D6-$C$6</f>
         <v>0</v>
       </c>
-      <c r="G6" s="61">
+      <c r="G6" s="110">
         <v>0</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="108">
         <v>0</v>
       </c>
       <c r="I6" s="3">
@@ -13095,30 +13129,30 @@
       <c r="J6" s="3">
         <v>70</v>
       </c>
-      <c r="K6" s="62">
+      <c r="K6" s="55">
         <f>J6-$I$6</f>
         <v>0</v>
       </c>
-      <c r="M6" s="65">
+      <c r="M6" s="110">
         <v>0</v>
       </c>
-      <c r="N6" s="79">
+      <c r="N6" s="113">
         <f>(B6+H6)/2</f>
         <v>0</v>
       </c>
-      <c r="P6" s="47">
+      <c r="Z6" s="45">
         <v>3.7499999999999999E-3</v>
       </c>
-      <c r="Q6" s="43">
+      <c r="AA6" s="41">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A7" s="110">
         <f>0.0003/(2*0.05)</f>
         <v>2.9999999999999996E-3</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="108">
         <f>E7/$C$6 *100</f>
         <v>-14.285714285714285</v>
       </c>
@@ -13130,11 +13164,11 @@
         <f t="shared" ref="E7:E13" si="0">D7-$C$6</f>
         <v>-30</v>
       </c>
-      <c r="G7" s="61">
+      <c r="G7" s="110">
         <f>0.0003/(2*0.05)</f>
         <v>2.9999999999999996E-3</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="108">
         <f>K7/$I$6 *100</f>
         <v>-4.2857142857142856</v>
       </c>
@@ -13142,30 +13176,31 @@
       <c r="J7" s="3">
         <v>67</v>
       </c>
-      <c r="K7" s="62">
+      <c r="K7" s="55">
         <f t="shared" ref="K7:K13" si="1">J7-$I$6</f>
         <v>-3</v>
       </c>
-      <c r="M7" s="65">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="N7" s="80">
+      <c r="M7" s="110">
+        <f>0.0003/(2*0.05)</f>
+        <v>2.9999999999999996E-3</v>
+      </c>
+      <c r="N7" s="114">
         <f t="shared" ref="N7:N13" si="2">(B7+H7)/2</f>
         <v>-9.2857142857142847</v>
       </c>
-      <c r="P7" s="47">
+      <c r="Z7" s="45">
         <v>4.2857140000000004E-3</v>
       </c>
-      <c r="Q7" s="43">
+      <c r="AA7" s="41">
         <v>3.5</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A8" s="110">
         <f>0.0003/(2*0.045)</f>
         <v>3.3333333333333331E-3</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="108">
         <f t="shared" ref="B8:B13" si="3">E8/$C$6 *100</f>
         <v>-20.476190476190474</v>
       </c>
@@ -13177,11 +13212,11 @@
         <f t="shared" si="0"/>
         <v>-43</v>
       </c>
-      <c r="G8" s="61">
+      <c r="G8" s="110">
         <f>0.0003/(2*0.045)</f>
         <v>3.3333333333333331E-3</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="108">
         <f t="shared" ref="H8:H13" si="4">K8/$I$6 *100</f>
         <v>-8.5714285714285712</v>
       </c>
@@ -13189,30 +13224,31 @@
       <c r="J8" s="3">
         <v>64</v>
       </c>
-      <c r="K8" s="62">
+      <c r="K8" s="55">
         <f t="shared" si="1"/>
         <v>-6</v>
       </c>
-      <c r="M8" s="65">
-        <v>3.333333E-3</v>
-      </c>
-      <c r="N8" s="80">
+      <c r="M8" s="110">
+        <f>0.0003/(2*0.045)</f>
+        <v>3.3333333333333331E-3</v>
+      </c>
+      <c r="N8" s="114">
         <f t="shared" si="2"/>
         <v>-14.523809523809522</v>
       </c>
-      <c r="P8" s="47">
+      <c r="Z8" s="45">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="Q8" s="43">
+      <c r="AA8" s="41">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A9" s="110">
         <f>0.0003/(2*0.04)</f>
         <v>3.7499999999999994E-3</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="108">
         <f t="shared" si="3"/>
         <v>-15.714285714285714</v>
       </c>
@@ -13224,11 +13260,11 @@
         <f t="shared" si="0"/>
         <v>-33</v>
       </c>
-      <c r="G9" s="61">
+      <c r="G9" s="110">
         <f>0.0003/(2*0.04)</f>
         <v>3.7499999999999994E-3</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="108">
         <f t="shared" si="4"/>
         <v>-2.8571428571428572</v>
       </c>
@@ -13236,30 +13272,31 @@
       <c r="J9" s="3">
         <v>68</v>
       </c>
-      <c r="K9" s="62">
+      <c r="K9" s="55">
         <f t="shared" si="1"/>
         <v>-2</v>
       </c>
-      <c r="M9" s="65">
-        <v>3.7499999999999999E-3</v>
-      </c>
-      <c r="N9" s="80">
+      <c r="M9" s="110">
+        <f>0.0003/(2*0.04)</f>
+        <v>3.7499999999999994E-3</v>
+      </c>
+      <c r="N9" s="114">
         <f t="shared" si="2"/>
         <v>-9.2857142857142847</v>
       </c>
-      <c r="P9" s="47">
+      <c r="Z9" s="45">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="Q9" s="43">
+      <c r="AA9" s="41">
         <v>2.5</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+    <row r="10" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="110">
         <f>0.0003/(2*0.035)</f>
         <v>4.2857142857142851E-3</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="108">
         <f t="shared" si="3"/>
         <v>-19.047619047619047</v>
       </c>
@@ -13271,11 +13308,11 @@
         <f t="shared" si="0"/>
         <v>-40</v>
       </c>
-      <c r="G10" s="61">
+      <c r="G10" s="110">
         <f>0.0003/(2*0.035)</f>
         <v>4.2857142857142851E-3</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="108">
         <f t="shared" si="4"/>
         <v>-25.714285714285712</v>
       </c>
@@ -13283,30 +13320,31 @@
       <c r="J10" s="3">
         <v>52</v>
       </c>
-      <c r="K10" s="62">
+      <c r="K10" s="55">
         <f t="shared" si="1"/>
         <v>-18</v>
       </c>
-      <c r="M10" s="65">
-        <v>4.2857140000000004E-3</v>
-      </c>
-      <c r="N10" s="80">
+      <c r="M10" s="110">
+        <f>0.0003/(2*0.035)</f>
+        <v>4.2857142857142851E-3</v>
+      </c>
+      <c r="N10" s="114">
         <f t="shared" si="2"/>
         <v>-22.38095238095238</v>
       </c>
-      <c r="P10" s="48">
+      <c r="Z10" s="46">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="Q10" s="45">
+      <c r="AA10" s="43">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A11" s="110">
         <f>0.0003/(2*0.03)</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="108">
         <f t="shared" si="3"/>
         <v>-12.380952380952381</v>
       </c>
@@ -13318,11 +13356,11 @@
         <f t="shared" si="0"/>
         <v>-26</v>
       </c>
-      <c r="G11" s="61">
+      <c r="G11" s="110">
         <f>0.0003/(2*0.03)</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="108">
         <f t="shared" si="4"/>
         <v>-32.857142857142854</v>
       </c>
@@ -13330,24 +13368,25 @@
       <c r="J11" s="3">
         <v>47</v>
       </c>
-      <c r="K11" s="62">
+      <c r="K11" s="55">
         <f t="shared" si="1"/>
         <v>-23</v>
       </c>
-      <c r="M11" s="65">
+      <c r="M11" s="110">
+        <f>0.0003/(2*0.03)</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="N11" s="80">
+      <c r="N11" s="114">
         <f t="shared" si="2"/>
         <v>-22.619047619047617</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A12" s="110">
         <f>0.0003/(2*0.025)</f>
         <v>5.9999999999999993E-3</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="108">
         <f t="shared" si="3"/>
         <v>-26.190476190476193</v>
       </c>
@@ -13359,11 +13398,11 @@
         <f t="shared" si="0"/>
         <v>-55</v>
       </c>
-      <c r="G12" s="61">
+      <c r="G12" s="110">
         <f>0.0003/(2*0.025)</f>
         <v>5.9999999999999993E-3</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="108">
         <f t="shared" si="4"/>
         <v>-42.857142857142854</v>
       </c>
@@ -13371,24 +13410,25 @@
       <c r="J12" s="3">
         <v>40</v>
       </c>
-      <c r="K12" s="62">
+      <c r="K12" s="55">
         <f t="shared" si="1"/>
         <v>-30</v>
       </c>
-      <c r="M12" s="65">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="N12" s="80">
+      <c r="M12" s="110">
+        <f>0.0003/(2*0.025)</f>
+        <v>5.9999999999999993E-3</v>
+      </c>
+      <c r="N12" s="114">
         <f t="shared" si="2"/>
         <v>-34.523809523809526</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+    <row r="13" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="111">
         <f>0.0003/(2*0.02)</f>
         <v>7.4999999999999989E-3</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="109">
         <f t="shared" si="3"/>
         <v>-28.571428571428569</v>
       </c>
@@ -13396,424 +13436,425 @@
       <c r="D13" s="4">
         <v>150</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="4">
         <f t="shared" si="0"/>
         <v>-60</v>
       </c>
-      <c r="G13" s="63">
+      <c r="G13" s="111">
         <f>0.0003/(2*0.02)</f>
         <v>7.4999999999999989E-3</v>
       </c>
-      <c r="H13" s="64">
+      <c r="H13" s="112">
         <f t="shared" si="4"/>
         <v>-41.428571428571431</v>
       </c>
-      <c r="I13" s="64"/>
-      <c r="J13" s="64">
+      <c r="I13" s="56"/>
+      <c r="J13" s="56">
         <v>41</v>
       </c>
-      <c r="K13" s="62">
+      <c r="K13" s="158">
         <f t="shared" si="1"/>
         <v>-29</v>
       </c>
-      <c r="M13" s="66">
-        <v>7.4999999999999997E-3</v>
-      </c>
-      <c r="N13" s="81">
+      <c r="M13" s="111">
+        <f>0.0003/(2*0.02)</f>
+        <v>7.4999999999999989E-3</v>
+      </c>
+      <c r="N13" s="115">
         <f t="shared" si="2"/>
         <v>-35</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="E14" s="7"/>
       <c r="G14" s="6"/>
       <c r="K14" s="7"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="51"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="49"/>
     </row>
-    <row r="15" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="104" t="s">
+    <row r="15" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="105"/>
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="106"/>
-      <c r="G15" s="104" t="s">
+      <c r="B15" s="99"/>
+      <c r="C15" s="99"/>
+      <c r="D15" s="99"/>
+      <c r="E15" s="100"/>
+      <c r="G15" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="105"/>
-      <c r="I15" s="105"/>
-      <c r="J15" s="105"/>
-      <c r="K15" s="106"/>
-      <c r="M15" s="121" t="s">
+      <c r="H15" s="99"/>
+      <c r="I15" s="99"/>
+      <c r="J15" s="99"/>
+      <c r="K15" s="100"/>
+      <c r="M15" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="N15" s="122"/>
+      <c r="N15" s="102"/>
     </row>
-    <row r="16" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+    <row r="16" spans="1:27" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="H16" s="70" t="s">
+      <c r="H16" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="I16" s="18" t="s">
+      <c r="I16" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="J16" s="19" t="s">
+      <c r="J16" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="K16" s="71" t="s">
+      <c r="K16" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="M16" s="52" t="s">
+      <c r="M16" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="N16" s="72" t="s">
+      <c r="N16" s="60" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="14">
+      <c r="A17" s="148">
         <v>0</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="122">
         <v>0</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="12">
         <v>300</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="8">
         <v>300</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="12">
         <f>D17-$C$17</f>
         <v>0</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="146">
         <v>0</v>
       </c>
-      <c r="H17" s="82">
+      <c r="H17" s="119">
         <v>0</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="9">
         <v>230</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17" s="8">
         <v>230</v>
       </c>
-      <c r="K17" s="132">
+      <c r="K17" s="68">
         <f>J17-$I$17</f>
         <v>0</v>
       </c>
-      <c r="M17" s="67">
+      <c r="M17" s="144">
         <v>0</v>
       </c>
-      <c r="N17" s="85">
+      <c r="N17" s="116">
         <f>(B17+H17)/2</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="14">
+      <c r="A18" s="148">
         <f>0.0003/(2*0.05)</f>
         <v>2.9999999999999996E-3</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="122">
         <f>E18/$C$17 *100</f>
         <v>-13.333333333333334</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="9">
+      <c r="C18" s="12"/>
+      <c r="D18" s="8">
         <v>260</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="12">
         <f t="shared" ref="E18:E24" si="5">D18-$C$17</f>
         <v>-40</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="146">
         <f>0.0003/(2*0.05)</f>
         <v>2.9999999999999996E-3</v>
       </c>
-      <c r="H18" s="83">
+      <c r="H18" s="120">
         <f>K18/$I$17 *100</f>
         <v>-7.8260869565217401</v>
       </c>
-      <c r="I18" s="10"/>
-      <c r="J18" s="9">
+      <c r="I18" s="9"/>
+      <c r="J18" s="8">
         <v>212</v>
       </c>
-      <c r="K18" s="14">
+      <c r="K18" s="12">
         <f t="shared" ref="K18:K24" si="6">J18-$I$17</f>
         <v>-18</v>
       </c>
-      <c r="M18" s="67">
+      <c r="M18" s="144">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="N18" s="86">
+      <c r="N18" s="117">
         <f t="shared" ref="N18:N24" si="7">(B18+H18)/2</f>
         <v>-10.579710144927537</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="14">
+      <c r="A19" s="148">
         <f>0.0003/(2*0.045)</f>
         <v>3.3333333333333331E-3</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="122">
         <f t="shared" ref="B19:B24" si="8">E19/$C$17 *100</f>
         <v>-14.333333333333334</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="9">
+      <c r="C19" s="12"/>
+      <c r="D19" s="8">
         <v>257</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="12">
         <f t="shared" si="5"/>
         <v>-43</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="146">
         <f>0.0003/(2*0.045)</f>
         <v>3.3333333333333331E-3</v>
       </c>
-      <c r="H19" s="83">
+      <c r="H19" s="120">
         <f t="shared" ref="H19:H24" si="9">K19/$I$17 *100</f>
         <v>-11.304347826086957</v>
       </c>
-      <c r="I19" s="10"/>
-      <c r="J19" s="9">
+      <c r="I19" s="9"/>
+      <c r="J19" s="8">
         <v>204</v>
       </c>
-      <c r="K19" s="14">
+      <c r="K19" s="12">
         <f t="shared" si="6"/>
         <v>-26</v>
       </c>
-      <c r="M19" s="67">
+      <c r="M19" s="144">
         <v>3.333333E-3</v>
       </c>
-      <c r="N19" s="86">
+      <c r="N19" s="117">
         <f t="shared" si="7"/>
         <v>-12.818840579710145</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="14">
+      <c r="A20" s="148">
         <f>0.0003/(2*0.04)</f>
         <v>3.7499999999999994E-3</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="122">
         <f t="shared" si="8"/>
         <v>-16.666666666666664</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="9">
+      <c r="C20" s="12"/>
+      <c r="D20" s="8">
         <v>250</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="12">
         <f t="shared" si="5"/>
         <v>-50</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="146">
         <f>0.0003/(2*0.04)</f>
         <v>3.7499999999999994E-3</v>
       </c>
-      <c r="H20" s="83">
+      <c r="H20" s="120">
         <f t="shared" si="9"/>
         <v>-15.217391304347828</v>
       </c>
-      <c r="I20" s="10"/>
-      <c r="J20" s="9">
+      <c r="I20" s="9"/>
+      <c r="J20" s="8">
         <v>195</v>
       </c>
-      <c r="K20" s="14">
+      <c r="K20" s="12">
         <f t="shared" si="6"/>
         <v>-35</v>
       </c>
-      <c r="M20" s="67">
+      <c r="M20" s="144">
         <v>3.7499999999999999E-3</v>
       </c>
-      <c r="N20" s="86">
+      <c r="N20" s="117">
         <f t="shared" si="7"/>
         <v>-15.942028985507246</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="14">
+      <c r="A21" s="148">
         <f>0.0003/(2*0.035)</f>
         <v>4.2857142857142851E-3</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="122">
         <f t="shared" si="8"/>
         <v>-26.666666666666668</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="9">
+      <c r="C21" s="12"/>
+      <c r="D21" s="8">
         <v>220</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="12">
         <f t="shared" si="5"/>
         <v>-80</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="146">
         <f>0.0003/(2*0.035)</f>
         <v>4.2857142857142851E-3</v>
       </c>
-      <c r="H21" s="83">
+      <c r="H21" s="120">
         <f t="shared" si="9"/>
         <v>-34.347826086956523</v>
       </c>
-      <c r="I21" s="10"/>
-      <c r="J21" s="9">
+      <c r="I21" s="9"/>
+      <c r="J21" s="8">
         <v>151</v>
       </c>
-      <c r="K21" s="14">
+      <c r="K21" s="12">
         <f t="shared" si="6"/>
         <v>-79</v>
       </c>
-      <c r="M21" s="67">
+      <c r="M21" s="144">
         <v>4.2857140000000004E-3</v>
       </c>
-      <c r="N21" s="86">
+      <c r="N21" s="117">
         <f t="shared" si="7"/>
         <v>-30.507246376811594</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="14">
+      <c r="A22" s="148">
         <f>0.0003/(2*0.03)</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="122">
         <f t="shared" si="8"/>
         <v>-30.333333333333336</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="9">
+      <c r="C22" s="12"/>
+      <c r="D22" s="8">
         <v>209</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="12">
         <f t="shared" si="5"/>
         <v>-91</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="146">
         <f>0.0003/(2*0.03)</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H22" s="83">
+      <c r="H22" s="120">
         <f t="shared" si="9"/>
         <v>-43.04347826086957</v>
       </c>
-      <c r="I22" s="10"/>
-      <c r="J22" s="9">
+      <c r="I22" s="9"/>
+      <c r="J22" s="8">
         <v>131</v>
       </c>
-      <c r="K22" s="14">
+      <c r="K22" s="12">
         <f t="shared" si="6"/>
         <v>-99</v>
       </c>
-      <c r="M22" s="67">
+      <c r="M22" s="144">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="N22" s="86">
+      <c r="N22" s="117">
         <f t="shared" si="7"/>
         <v>-36.688405797101453</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="14">
+      <c r="A23" s="148">
         <f>0.0003/(2*0.025)</f>
         <v>5.9999999999999993E-3</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="122">
         <f t="shared" si="8"/>
         <v>-36.666666666666664</v>
       </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="9">
+      <c r="C23" s="12"/>
+      <c r="D23" s="8">
         <v>190</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="12">
         <f t="shared" si="5"/>
         <v>-110</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="146">
         <f>0.0003/(2*0.025)</f>
         <v>5.9999999999999993E-3</v>
       </c>
-      <c r="H23" s="83">
+      <c r="H23" s="120">
         <f t="shared" si="9"/>
         <v>-47.826086956521742</v>
       </c>
-      <c r="I23" s="10"/>
-      <c r="J23" s="9">
+      <c r="I23" s="9"/>
+      <c r="J23" s="8">
         <v>120</v>
       </c>
-      <c r="K23" s="14">
+      <c r="K23" s="12">
         <f t="shared" si="6"/>
         <v>-110</v>
       </c>
-      <c r="M23" s="67">
+      <c r="M23" s="144">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="N23" s="86">
+      <c r="N23" s="117">
         <f t="shared" si="7"/>
         <v>-42.246376811594203</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15">
+      <c r="A24" s="149">
         <f>0.0003/(2*0.02)</f>
         <v>7.4999999999999989E-3</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="123">
         <f t="shared" si="8"/>
         <v>-42</v>
       </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="12">
+      <c r="C24" s="13"/>
+      <c r="D24" s="10">
         <v>174</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24" s="13">
         <f t="shared" si="5"/>
         <v>-126</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G24" s="147">
         <f>0.0003/(2*0.02)</f>
         <v>7.4999999999999989E-3</v>
       </c>
-      <c r="H24" s="84">
+      <c r="H24" s="121">
         <f t="shared" si="9"/>
         <v>-55.652173913043477</v>
       </c>
-      <c r="I24" s="13"/>
-      <c r="J24" s="12">
+      <c r="I24" s="11"/>
+      <c r="J24" s="10">
         <v>102</v>
       </c>
-      <c r="K24" s="15">
+      <c r="K24" s="13">
         <f t="shared" si="6"/>
         <v>-128</v>
       </c>
-      <c r="M24" s="68">
+      <c r="M24" s="145">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="N24" s="87">
+      <c r="N24" s="118">
         <f t="shared" si="7"/>
         <v>-48.826086956521735</v>
       </c>
@@ -13823,391 +13864,391 @@
       <c r="E25" s="7"/>
       <c r="G25" s="6"/>
       <c r="K25" s="7"/>
-      <c r="M25" s="50"/>
-      <c r="N25" s="51"/>
+      <c r="M25" s="48"/>
+      <c r="N25" s="49"/>
     </row>
     <row r="26" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="110" t="s">
+      <c r="A26" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="111"/>
-      <c r="C26" s="111"/>
-      <c r="D26" s="111"/>
-      <c r="E26" s="112"/>
-      <c r="G26" s="110" t="s">
+      <c r="B26" s="94"/>
+      <c r="C26" s="94"/>
+      <c r="D26" s="94"/>
+      <c r="E26" s="95"/>
+      <c r="G26" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="H26" s="111"/>
-      <c r="I26" s="111"/>
-      <c r="J26" s="111"/>
-      <c r="K26" s="112"/>
-      <c r="M26" s="125" t="s">
+      <c r="H26" s="94"/>
+      <c r="I26" s="94"/>
+      <c r="J26" s="94"/>
+      <c r="K26" s="95"/>
+      <c r="M26" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="N26" s="126"/>
+      <c r="N26" s="97"/>
     </row>
     <row r="27" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="33" t="s">
+      <c r="B27" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="31" t="s">
+      <c r="C27" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="33" t="s">
+      <c r="D27" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="32" t="s">
+      <c r="E27" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="G27" s="30" t="s">
+      <c r="G27" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="H27" s="76" t="s">
+      <c r="H27" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="I27" s="31" t="s">
+      <c r="I27" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="J27" s="33" t="s">
+      <c r="J27" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="K27" s="75" t="s">
+      <c r="K27" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="M27" s="56" t="s">
+      <c r="M27" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="N27" s="74" t="s">
+      <c r="N27" s="62" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="36">
+      <c r="A28" s="156">
         <v>0</v>
       </c>
-      <c r="B28" s="34">
+      <c r="B28" s="132">
         <v>0</v>
       </c>
-      <c r="C28" s="29">
+      <c r="C28" s="27">
         <v>150</v>
       </c>
-      <c r="D28" s="34">
+      <c r="D28" s="32">
         <v>150</v>
       </c>
-      <c r="E28" s="37">
+      <c r="E28" s="35">
         <f>D28-$C$28</f>
         <v>0</v>
       </c>
-      <c r="G28" s="36">
+      <c r="G28" s="156">
         <v>0</v>
       </c>
-      <c r="H28" s="94">
+      <c r="H28" s="134">
         <v>0</v>
       </c>
-      <c r="I28" s="29">
+      <c r="I28" s="27">
         <v>200</v>
       </c>
-      <c r="J28" s="36">
+      <c r="J28" s="34">
         <v>200</v>
       </c>
-      <c r="K28" s="133">
+      <c r="K28" s="69">
         <f>J28-$I$28</f>
         <v>0</v>
       </c>
-      <c r="M28" s="57">
+      <c r="M28" s="154">
         <v>0</v>
       </c>
-      <c r="N28" s="91">
+      <c r="N28" s="137">
         <f>(B28+H28)/2</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="36">
+      <c r="A29" s="156">
         <f>0.0003/(2*0.05)</f>
         <v>2.9999999999999996E-3</v>
       </c>
-      <c r="B29" s="34">
+      <c r="B29" s="132">
         <f>E29/$C$28 *100</f>
         <v>-12.666666666666668</v>
       </c>
-      <c r="C29" s="29"/>
-      <c r="D29" s="34">
+      <c r="C29" s="27"/>
+      <c r="D29" s="32">
         <v>131</v>
       </c>
-      <c r="E29" s="37">
+      <c r="E29" s="35">
         <f t="shared" ref="E29:E35" si="10">D29-$C$28</f>
         <v>-19</v>
       </c>
-      <c r="G29" s="36">
+      <c r="G29" s="156">
         <f>0.0003/(2*0.05)</f>
         <v>2.9999999999999996E-3</v>
       </c>
-      <c r="H29" s="95">
+      <c r="H29" s="135">
         <f>K29/$I$28 *100</f>
         <v>-4</v>
       </c>
-      <c r="I29" s="29"/>
-      <c r="J29" s="36">
+      <c r="I29" s="27"/>
+      <c r="J29" s="34">
         <v>192</v>
       </c>
-      <c r="K29" s="34">
+      <c r="K29" s="32">
         <f t="shared" ref="K29:K35" si="11">J29-$I$28</f>
         <v>-8</v>
       </c>
-      <c r="M29" s="57">
+      <c r="M29" s="154">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="N29" s="92">
+      <c r="N29" s="138">
         <f t="shared" ref="N29:N35" si="12">(B29+H29)/2</f>
         <v>-8.3333333333333339</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="36">
+      <c r="A30" s="156">
         <f>0.0003/(2*0.045)</f>
         <v>3.3333333333333331E-3</v>
       </c>
-      <c r="B30" s="34">
+      <c r="B30" s="132">
         <f t="shared" ref="B30:B35" si="13">E30/$C$28 *100</f>
         <v>-18</v>
       </c>
-      <c r="C30" s="29"/>
-      <c r="D30" s="34">
+      <c r="C30" s="27"/>
+      <c r="D30" s="32">
         <v>123</v>
       </c>
-      <c r="E30" s="37">
+      <c r="E30" s="35">
         <f t="shared" si="10"/>
         <v>-27</v>
       </c>
-      <c r="G30" s="36">
+      <c r="G30" s="156">
         <f>0.0003/(2*0.045)</f>
         <v>3.3333333333333331E-3</v>
       </c>
-      <c r="H30" s="95">
+      <c r="H30" s="135">
         <f t="shared" ref="H30:H35" si="14">K30/$I$28 *100</f>
         <v>-11.5</v>
       </c>
-      <c r="I30" s="29"/>
-      <c r="J30" s="36">
+      <c r="I30" s="27"/>
+      <c r="J30" s="34">
         <v>177</v>
       </c>
-      <c r="K30" s="34">
+      <c r="K30" s="32">
         <f t="shared" si="11"/>
         <v>-23</v>
       </c>
-      <c r="M30" s="57">
+      <c r="M30" s="154">
         <v>3.333333E-3</v>
       </c>
-      <c r="N30" s="92">
+      <c r="N30" s="138">
         <f t="shared" si="12"/>
         <v>-14.75</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="36">
+      <c r="A31" s="156">
         <f>0.0003/(2*0.04)</f>
         <v>3.7499999999999994E-3</v>
       </c>
-      <c r="B31" s="34">
+      <c r="B31" s="132">
         <f t="shared" si="13"/>
         <v>-20</v>
       </c>
-      <c r="C31" s="29"/>
-      <c r="D31" s="34">
+      <c r="C31" s="27"/>
+      <c r="D31" s="32">
         <v>120</v>
       </c>
-      <c r="E31" s="37">
+      <c r="E31" s="35">
         <f t="shared" si="10"/>
         <v>-30</v>
       </c>
-      <c r="G31" s="36">
+      <c r="G31" s="156">
         <f>0.0003/(2*0.04)</f>
         <v>3.7499999999999994E-3</v>
       </c>
-      <c r="H31" s="95">
+      <c r="H31" s="135">
         <f t="shared" si="14"/>
         <v>-8.5</v>
       </c>
-      <c r="I31" s="29"/>
-      <c r="J31" s="36">
+      <c r="I31" s="27"/>
+      <c r="J31" s="34">
         <v>183</v>
       </c>
-      <c r="K31" s="34">
+      <c r="K31" s="32">
         <f t="shared" si="11"/>
         <v>-17</v>
       </c>
-      <c r="M31" s="57">
+      <c r="M31" s="154">
         <v>3.7499999999999999E-3</v>
       </c>
-      <c r="N31" s="92">
+      <c r="N31" s="138">
         <f t="shared" si="12"/>
         <v>-14.25</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="36">
+      <c r="A32" s="156">
         <f>0.0003/(2*0.035)</f>
         <v>4.2857142857142851E-3</v>
       </c>
-      <c r="B32" s="34">
+      <c r="B32" s="132">
         <f t="shared" si="13"/>
         <v>-22</v>
       </c>
-      <c r="C32" s="29"/>
-      <c r="D32" s="34">
+      <c r="C32" s="27"/>
+      <c r="D32" s="32">
         <v>117</v>
       </c>
-      <c r="E32" s="37">
+      <c r="E32" s="35">
         <f t="shared" si="10"/>
         <v>-33</v>
       </c>
-      <c r="G32" s="36">
+      <c r="G32" s="156">
         <f>0.0003/(2*0.035)</f>
         <v>4.2857142857142851E-3</v>
       </c>
-      <c r="H32" s="95">
+      <c r="H32" s="135">
         <f t="shared" si="14"/>
         <v>-18</v>
       </c>
-      <c r="I32" s="29"/>
-      <c r="J32" s="36">
+      <c r="I32" s="27"/>
+      <c r="J32" s="34">
         <v>164</v>
       </c>
-      <c r="K32" s="34">
+      <c r="K32" s="32">
         <f t="shared" si="11"/>
         <v>-36</v>
       </c>
-      <c r="M32" s="57">
+      <c r="M32" s="154">
         <v>4.2857140000000004E-3</v>
       </c>
-      <c r="N32" s="92">
+      <c r="N32" s="138">
         <f t="shared" si="12"/>
         <v>-20</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33" s="36">
+      <c r="A33" s="156">
         <f>0.0003/(2*0.03)</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="B33" s="34">
+      <c r="B33" s="132">
         <f t="shared" si="13"/>
         <v>-20</v>
       </c>
-      <c r="C33" s="29"/>
-      <c r="D33" s="34">
+      <c r="C33" s="27"/>
+      <c r="D33" s="32">
         <v>120</v>
       </c>
-      <c r="E33" s="37">
+      <c r="E33" s="35">
         <f t="shared" si="10"/>
         <v>-30</v>
       </c>
-      <c r="G33" s="36">
+      <c r="G33" s="156">
         <f>0.0003/(2*0.03)</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H33" s="95">
+      <c r="H33" s="135">
         <f t="shared" si="14"/>
         <v>-28.499999999999996</v>
       </c>
-      <c r="I33" s="29"/>
-      <c r="J33" s="36">
+      <c r="I33" s="27"/>
+      <c r="J33" s="34">
         <v>143</v>
       </c>
-      <c r="K33" s="34">
+      <c r="K33" s="32">
         <f t="shared" si="11"/>
         <v>-57</v>
       </c>
-      <c r="M33" s="57">
+      <c r="M33" s="154">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="N33" s="92">
+      <c r="N33" s="138">
         <f t="shared" si="12"/>
         <v>-24.25</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A34" s="36">
+      <c r="A34" s="156">
         <f>0.0003/(2*0.025)</f>
         <v>5.9999999999999993E-3</v>
       </c>
-      <c r="B34" s="34">
+      <c r="B34" s="132">
         <f t="shared" si="13"/>
         <v>-28.666666666666668</v>
       </c>
-      <c r="C34" s="29"/>
-      <c r="D34" s="34">
+      <c r="C34" s="27"/>
+      <c r="D34" s="32">
         <v>107</v>
       </c>
-      <c r="E34" s="37">
+      <c r="E34" s="35">
         <f t="shared" si="10"/>
         <v>-43</v>
       </c>
-      <c r="G34" s="36">
+      <c r="G34" s="156">
         <f>0.0003/(2*0.025)</f>
         <v>5.9999999999999993E-3</v>
       </c>
-      <c r="H34" s="95">
+      <c r="H34" s="135">
         <f t="shared" si="14"/>
         <v>-39.5</v>
       </c>
-      <c r="I34" s="29"/>
-      <c r="J34" s="36">
+      <c r="I34" s="27"/>
+      <c r="J34" s="34">
         <v>121</v>
       </c>
-      <c r="K34" s="34">
+      <c r="K34" s="32">
         <f t="shared" si="11"/>
         <v>-79</v>
       </c>
-      <c r="M34" s="57">
+      <c r="M34" s="154">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="N34" s="92">
+      <c r="N34" s="138">
         <f t="shared" si="12"/>
         <v>-34.083333333333336</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="38">
+      <c r="A35" s="157">
         <f>0.0003/(2*0.02)</f>
         <v>7.4999999999999989E-3</v>
       </c>
-      <c r="B35" s="35">
+      <c r="B35" s="133">
         <f t="shared" si="13"/>
         <v>-38.666666666666664</v>
       </c>
-      <c r="C35" s="39"/>
-      <c r="D35" s="35">
+      <c r="C35" s="37"/>
+      <c r="D35" s="33">
         <v>92</v>
       </c>
-      <c r="E35" s="37">
+      <c r="E35" s="33">
         <f t="shared" si="10"/>
         <v>-58</v>
       </c>
-      <c r="G35" s="38">
+      <c r="G35" s="157">
         <f>0.0003/(2*0.02)</f>
         <v>7.4999999999999989E-3</v>
       </c>
-      <c r="H35" s="96">
+      <c r="H35" s="136">
         <f t="shared" si="14"/>
         <v>-45</v>
       </c>
-      <c r="I35" s="39"/>
-      <c r="J35" s="38">
+      <c r="I35" s="37"/>
+      <c r="J35" s="36">
         <v>110</v>
       </c>
-      <c r="K35" s="35">
+      <c r="K35" s="33">
         <f t="shared" si="11"/>
         <v>-90</v>
       </c>
-      <c r="M35" s="58">
+      <c r="M35" s="155">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="N35" s="93">
+      <c r="N35" s="139">
         <f t="shared" si="12"/>
         <v>-41.833333333333329</v>
       </c>
@@ -14235,10 +14276,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A9BAF04-6FC7-CE48-AE14-9D2C2252560B}">
-  <dimension ref="A1:Q46"/>
+  <dimension ref="A1:AA46"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A77" sqref="A62:J77"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14262,872 +14303,872 @@
     <col min="18" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="113" t="s">
+    <row r="1" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
-      <c r="D1" s="114"/>
-      <c r="E1" s="115"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="79"/>
     </row>
-    <row r="2" spans="1:17" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="P2" s="41" t="s">
+    <row r="2" spans="1:27" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="Z2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="100" t="s">
+      <c r="AA2" s="67" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="116" t="s">
+    <row r="3" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="117"/>
-      <c r="C3" s="117"/>
-      <c r="D3" s="117"/>
-      <c r="E3" s="118"/>
-      <c r="G3" s="127" t="s">
+      <c r="B3" s="81"/>
+      <c r="C3" s="81"/>
+      <c r="D3" s="81"/>
+      <c r="E3" s="82"/>
+      <c r="G3" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="128"/>
-      <c r="I3" s="128"/>
-      <c r="J3" s="128"/>
-      <c r="K3" s="129"/>
-      <c r="M3" s="127" t="s">
+      <c r="H3" s="84"/>
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="85"/>
+      <c r="M3" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="129"/>
-      <c r="P3" s="46">
+      <c r="N3" s="85"/>
+      <c r="Z3" s="44">
         <v>0</v>
       </c>
-      <c r="Q3" s="42" t="s">
+      <c r="AA3" s="40" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="101" t="s">
+    <row r="4" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="102"/>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="103"/>
-      <c r="G4" s="130" t="s">
+      <c r="B4" s="87"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="87"/>
+      <c r="E4" s="88"/>
+      <c r="G4" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
-      <c r="J4" s="102"/>
-      <c r="K4" s="131"/>
-      <c r="M4" s="119" t="s">
+      <c r="H4" s="87"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="87"/>
+      <c r="K4" s="90"/>
+      <c r="M4" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="120"/>
-      <c r="P4" s="47">
+      <c r="N4" s="92"/>
+      <c r="Z4" s="45">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="Q4" s="43">
+      <c r="AA4" s="41">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:27" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="137" t="s">
+      <c r="E5" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="59" t="s">
+      <c r="G5" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="138" t="s">
+      <c r="K5" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="49" t="s">
+      <c r="M5" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="N5" s="69" t="s">
+      <c r="N5" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="47">
+      <c r="Z5" s="45">
         <v>3.333333E-3</v>
       </c>
-      <c r="Q5" s="44">
+      <c r="AA5" s="42">
         <v>4.5</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A6" s="110">
         <v>0</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="108">
         <v>0</v>
       </c>
       <c r="C6" s="3">
         <v>140</v>
       </c>
-      <c r="D6" s="134">
+      <c r="D6" s="70">
         <v>140</v>
       </c>
-      <c r="E6" s="139">
+      <c r="E6" s="75">
         <f>D6-$C$6</f>
         <v>0</v>
       </c>
-      <c r="G6" s="61">
+      <c r="G6" s="140">
         <v>0</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="108">
         <v>0</v>
       </c>
       <c r="I6" s="3">
         <v>42</v>
       </c>
-      <c r="J6" s="134">
+      <c r="J6" s="70">
         <v>42</v>
       </c>
-      <c r="K6" s="139">
+      <c r="K6" s="75">
         <f>J6-$I$6</f>
         <v>0</v>
       </c>
-      <c r="M6" s="65">
+      <c r="M6" s="142">
         <v>0</v>
       </c>
-      <c r="N6" s="79">
+      <c r="N6" s="113">
         <f>(B6+H6)/2</f>
         <v>0</v>
       </c>
-      <c r="P6" s="47">
+      <c r="Z6" s="45">
         <v>3.7499999999999999E-3</v>
       </c>
-      <c r="Q6" s="43">
+      <c r="AA6" s="41">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A7" s="110">
         <f>0.0003/(2*0.05)</f>
         <v>2.9999999999999996E-3</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="108">
         <f>E7/$C$6 *100</f>
         <v>2.1428571428571428</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="134">
+      <c r="D7" s="70">
         <v>143</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" ref="E7:E13" si="0">D7-$C$6</f>
         <v>3</v>
       </c>
-      <c r="G7" s="61">
+      <c r="G7" s="140">
         <f>0.0003/(2*0.05)</f>
         <v>2.9999999999999996E-3</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="108">
         <f>K7/$I$6 *100</f>
         <v>4.7619047619047619</v>
       </c>
       <c r="I7" s="3"/>
-      <c r="J7" s="134">
+      <c r="J7" s="70">
         <v>44</v>
       </c>
       <c r="K7" s="3">
         <f t="shared" ref="K7:K13" si="1">J7-$I$6</f>
         <v>2</v>
       </c>
-      <c r="M7" s="65">
+      <c r="M7" s="142">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="N7" s="80">
+      <c r="N7" s="114">
         <f t="shared" ref="N7:N13" si="2">(B7+H7)/2</f>
         <v>3.4523809523809526</v>
       </c>
-      <c r="P7" s="47">
+      <c r="Z7" s="45">
         <v>4.2857140000000004E-3</v>
       </c>
-      <c r="Q7" s="43">
+      <c r="AA7" s="41">
         <v>3.5</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A8" s="110">
         <f>0.0003/(2*0.045)</f>
         <v>3.3333333333333331E-3</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="108">
         <f t="shared" ref="B8:B13" si="3">E8/$C$6 *100</f>
         <v>5.7142857142857144</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="134">
+      <c r="D8" s="70">
         <v>148</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G8" s="61">
+      <c r="G8" s="140">
         <f>0.0003/(2*0.045)</f>
         <v>3.3333333333333331E-3</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="108">
         <f t="shared" ref="H8:H13" si="4">K8/$I$6 *100</f>
         <v>4.7619047619047619</v>
       </c>
       <c r="I8" s="3"/>
-      <c r="J8" s="134">
+      <c r="J8" s="70">
         <v>44</v>
       </c>
       <c r="K8" s="3">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M8" s="65">
+      <c r="M8" s="142">
         <v>3.333333E-3</v>
       </c>
-      <c r="N8" s="80">
+      <c r="N8" s="114">
         <f t="shared" si="2"/>
         <v>5.2380952380952381</v>
       </c>
-      <c r="P8" s="47">
+      <c r="Z8" s="45">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="Q8" s="43">
+      <c r="AA8" s="41">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A9" s="110">
         <f>0.0003/(2*0.04)</f>
         <v>3.7499999999999994E-3</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="108">
         <f t="shared" si="3"/>
         <v>7.8571428571428568</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="134">
+      <c r="D9" s="70">
         <v>151</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="G9" s="61">
+      <c r="G9" s="140">
         <f>0.0003/(2*0.04)</f>
         <v>3.7499999999999994E-3</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="108">
         <f t="shared" si="4"/>
         <v>19.047619047619047</v>
       </c>
       <c r="I9" s="3"/>
-      <c r="J9" s="134">
+      <c r="J9" s="70">
         <v>50</v>
       </c>
       <c r="K9" s="3">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="M9" s="65">
+      <c r="M9" s="142">
         <v>3.7499999999999999E-3</v>
       </c>
-      <c r="N9" s="80">
+      <c r="N9" s="114">
         <f t="shared" si="2"/>
         <v>13.452380952380953</v>
       </c>
-      <c r="P9" s="47">
+      <c r="Z9" s="45">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="Q9" s="43">
+      <c r="AA9" s="41">
         <v>2.5</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+    <row r="10" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="110">
         <f>0.0003/(2*0.035)</f>
         <v>4.2857142857142851E-3</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="108">
         <f t="shared" si="3"/>
         <v>10.714285714285714</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="134">
+      <c r="D10" s="70">
         <v>155</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G10" s="61">
+      <c r="G10" s="140">
         <f>0.0003/(2*0.035)</f>
         <v>4.2857142857142851E-3</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="108">
         <f t="shared" si="4"/>
         <v>14.285714285714285</v>
       </c>
       <c r="I10" s="3"/>
-      <c r="J10" s="134">
+      <c r="J10" s="70">
         <v>48</v>
       </c>
       <c r="K10" s="3">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="M10" s="65">
+      <c r="M10" s="142">
         <v>4.2857140000000004E-3</v>
       </c>
-      <c r="N10" s="80">
+      <c r="N10" s="114">
         <f t="shared" si="2"/>
         <v>12.5</v>
       </c>
-      <c r="P10" s="48">
+      <c r="Z10" s="46">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="Q10" s="45">
+      <c r="AA10" s="43">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A11" s="110">
         <f>0.0003/(2*0.03)</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="108">
         <f t="shared" si="3"/>
         <v>14.285714285714285</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="134">
+      <c r="D11" s="70">
         <v>160</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="G11" s="61">
+      <c r="G11" s="140">
         <f>0.0003/(2*0.03)</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="108">
         <f t="shared" si="4"/>
         <v>30.952380952380953</v>
       </c>
       <c r="I11" s="3"/>
-      <c r="J11" s="134">
+      <c r="J11" s="70">
         <v>55</v>
       </c>
       <c r="K11" s="3">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="M11" s="65">
+      <c r="M11" s="142">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="N11" s="80">
+      <c r="N11" s="114">
         <f t="shared" si="2"/>
         <v>22.61904761904762</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A12" s="110">
         <f>0.0003/(2*0.025)</f>
         <v>5.9999999999999993E-3</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="108">
         <f t="shared" si="3"/>
         <v>16.428571428571427</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="134">
+      <c r="D12" s="70">
         <v>163</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="G12" s="61">
+      <c r="G12" s="140">
         <f>0.0003/(2*0.025)</f>
         <v>5.9999999999999993E-3</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="108">
         <f t="shared" si="4"/>
         <v>38.095238095238095</v>
       </c>
       <c r="I12" s="3"/>
-      <c r="J12" s="134">
+      <c r="J12" s="70">
         <v>58</v>
       </c>
       <c r="K12" s="3">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="M12" s="65">
+      <c r="M12" s="142">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="N12" s="80">
+      <c r="N12" s="114">
         <f t="shared" si="2"/>
         <v>27.261904761904759</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+    <row r="13" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="111">
         <f>0.0003/(2*0.02)</f>
         <v>7.4999999999999989E-3</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="109">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13" s="135">
+      <c r="D13" s="71">
         <v>168</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="G13" s="63">
+      <c r="G13" s="141">
         <f>0.0003/(2*0.02)</f>
         <v>7.4999999999999989E-3</v>
       </c>
-      <c r="H13" s="64">
+      <c r="H13" s="112">
         <f t="shared" si="4"/>
         <v>38.095238095238095</v>
       </c>
-      <c r="I13" s="64"/>
-      <c r="J13" s="136">
+      <c r="I13" s="56"/>
+      <c r="J13" s="72">
         <v>58</v>
       </c>
       <c r="K13" s="4">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="M13" s="66">
+      <c r="M13" s="143">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="N13" s="81">
+      <c r="N13" s="115">
         <f t="shared" si="2"/>
         <v>29.047619047619047</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="E14" s="7"/>
       <c r="G14" s="6"/>
       <c r="K14" s="7"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="51"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="49"/>
     </row>
-    <row r="15" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="104" t="s">
+    <row r="15" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="105"/>
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="106"/>
-      <c r="G15" s="104" t="s">
+      <c r="B15" s="99"/>
+      <c r="C15" s="99"/>
+      <c r="D15" s="99"/>
+      <c r="E15" s="100"/>
+      <c r="G15" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="105"/>
-      <c r="I15" s="105"/>
-      <c r="J15" s="105"/>
-      <c r="K15" s="106"/>
-      <c r="M15" s="121" t="s">
+      <c r="H15" s="99"/>
+      <c r="I15" s="99"/>
+      <c r="J15" s="99"/>
+      <c r="K15" s="100"/>
+      <c r="M15" s="101" t="s">
         <v>6</v>
       </c>
-      <c r="N15" s="122"/>
+      <c r="N15" s="102"/>
     </row>
-    <row r="16" spans="1:17" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+    <row r="16" spans="1:27" s="5" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E16" s="71" t="s">
+      <c r="E16" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="H16" s="70" t="s">
+      <c r="H16" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="I16" s="18" t="s">
+      <c r="I16" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="J16" s="19" t="s">
+      <c r="J16" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="K16" s="71" t="s">
+      <c r="K16" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="M16" s="52" t="s">
+      <c r="M16" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="N16" s="72" t="s">
+      <c r="N16" s="60" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A17" s="14">
+      <c r="A17" s="148">
         <v>0</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="122">
         <v>0</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="12">
         <v>180</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="8">
         <v>180</v>
       </c>
-      <c r="E17" s="132">
+      <c r="E17" s="68">
         <f>D17-$C$17</f>
         <v>0</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="146">
         <v>0</v>
       </c>
-      <c r="H17" s="82">
+      <c r="H17" s="119">
         <v>0</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="9">
         <v>200</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17" s="8">
         <v>200</v>
       </c>
-      <c r="K17" s="132">
+      <c r="K17" s="68">
         <f>J17-$I$17</f>
         <v>0</v>
       </c>
-      <c r="M17" s="67">
+      <c r="M17" s="144">
         <v>0</v>
       </c>
-      <c r="N17" s="85">
+      <c r="N17" s="116">
         <f>(B17+H17)/2</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A18" s="14">
+      <c r="A18" s="148">
         <f>0.0003/(2*0.05)</f>
         <v>2.9999999999999996E-3</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="122">
         <f>E18/$C$17 *100</f>
         <v>18.333333333333332</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="9">
+      <c r="C18" s="12"/>
+      <c r="D18" s="8">
         <v>213</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="12">
         <f t="shared" ref="E18:E24" si="5">D18-$C$17</f>
         <v>33</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="146">
         <f>0.0003/(2*0.05)</f>
         <v>2.9999999999999996E-3</v>
       </c>
-      <c r="H18" s="83">
+      <c r="H18" s="120">
         <f>K18/$I$17 *100</f>
         <v>14.499999999999998</v>
       </c>
-      <c r="I18" s="10"/>
-      <c r="J18" s="9">
+      <c r="I18" s="9"/>
+      <c r="J18" s="8">
         <v>229</v>
       </c>
-      <c r="K18" s="14">
+      <c r="K18" s="12">
         <f t="shared" ref="K18:K24" si="6">J18-$I$17</f>
         <v>29</v>
       </c>
-      <c r="M18" s="67">
+      <c r="M18" s="144">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="N18" s="86">
+      <c r="N18" s="117">
         <f t="shared" ref="N18:N24" si="7">(B18+H18)/2</f>
         <v>16.416666666666664</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="14">
+      <c r="A19" s="148">
         <f>0.0003/(2*0.045)</f>
         <v>3.3333333333333331E-3</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="122">
         <f t="shared" ref="B19:B24" si="8">E19/$C$17 *100</f>
         <v>22.222222222222221</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="9">
+      <c r="C19" s="12"/>
+      <c r="D19" s="8">
         <v>220</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="12">
         <f t="shared" si="5"/>
         <v>40</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="146">
         <f>0.0003/(2*0.045)</f>
         <v>3.3333333333333331E-3</v>
       </c>
-      <c r="H19" s="83">
+      <c r="H19" s="120">
         <f t="shared" ref="H19:H24" si="9">K19/$I$17 *100</f>
         <v>16.5</v>
       </c>
-      <c r="I19" s="10"/>
-      <c r="J19" s="9">
+      <c r="I19" s="9"/>
+      <c r="J19" s="8">
         <v>233</v>
       </c>
-      <c r="K19" s="14">
+      <c r="K19" s="12">
         <f t="shared" si="6"/>
         <v>33</v>
       </c>
-      <c r="M19" s="67">
+      <c r="M19" s="144">
         <v>3.333333E-3</v>
       </c>
-      <c r="N19" s="86">
+      <c r="N19" s="117">
         <f t="shared" si="7"/>
         <v>19.361111111111111</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="14">
+      <c r="A20" s="148">
         <f>0.0003/(2*0.04)</f>
         <v>3.7499999999999994E-3</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="122">
         <f t="shared" si="8"/>
         <v>25</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="9">
+      <c r="C20" s="12"/>
+      <c r="D20" s="8">
         <v>225</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="12">
         <f t="shared" si="5"/>
         <v>45</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="146">
         <f>0.0003/(2*0.04)</f>
         <v>3.7499999999999994E-3</v>
       </c>
-      <c r="H20" s="83">
+      <c r="H20" s="120">
         <f t="shared" si="9"/>
         <v>24.5</v>
       </c>
-      <c r="I20" s="10"/>
-      <c r="J20" s="9">
+      <c r="I20" s="9"/>
+      <c r="J20" s="8">
         <v>249</v>
       </c>
-      <c r="K20" s="14">
+      <c r="K20" s="12">
         <f t="shared" si="6"/>
         <v>49</v>
       </c>
-      <c r="M20" s="67">
+      <c r="M20" s="144">
         <v>3.7499999999999999E-3</v>
       </c>
-      <c r="N20" s="86">
+      <c r="N20" s="117">
         <f t="shared" si="7"/>
         <v>24.75</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="14">
+      <c r="A21" s="148">
         <f>0.0003/(2*0.035)</f>
         <v>4.2857142857142851E-3</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="122">
         <f t="shared" si="8"/>
         <v>28.888888888888886</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="9">
+      <c r="C21" s="12"/>
+      <c r="D21" s="8">
         <v>232</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="12">
         <f t="shared" si="5"/>
         <v>52</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="146">
         <f>0.0003/(2*0.035)</f>
         <v>4.2857142857142851E-3</v>
       </c>
-      <c r="H21" s="83">
+      <c r="H21" s="120">
         <f t="shared" si="9"/>
         <v>27.500000000000004</v>
       </c>
-      <c r="I21" s="10"/>
-      <c r="J21" s="9">
+      <c r="I21" s="9"/>
+      <c r="J21" s="8">
         <v>255</v>
       </c>
-      <c r="K21" s="14">
+      <c r="K21" s="12">
         <f t="shared" si="6"/>
         <v>55</v>
       </c>
-      <c r="M21" s="67">
+      <c r="M21" s="144">
         <v>4.2857140000000004E-3</v>
       </c>
-      <c r="N21" s="86">
+      <c r="N21" s="117">
         <f t="shared" si="7"/>
         <v>28.194444444444443</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="14">
+      <c r="A22" s="148">
         <f>0.0003/(2*0.03)</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="122">
         <f t="shared" si="8"/>
         <v>36.111111111111107</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="9">
+      <c r="C22" s="12"/>
+      <c r="D22" s="8">
         <v>245</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="12">
         <f t="shared" si="5"/>
         <v>65</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="146">
         <f>0.0003/(2*0.03)</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H22" s="83">
+      <c r="H22" s="120">
         <f t="shared" si="9"/>
         <v>38</v>
       </c>
-      <c r="I22" s="10"/>
-      <c r="J22" s="9">
+      <c r="I22" s="9"/>
+      <c r="J22" s="8">
         <v>276</v>
       </c>
-      <c r="K22" s="14">
+      <c r="K22" s="12">
         <f t="shared" si="6"/>
         <v>76</v>
       </c>
-      <c r="M22" s="67">
+      <c r="M22" s="144">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="N22" s="86">
+      <c r="N22" s="117">
         <f t="shared" si="7"/>
         <v>37.055555555555557</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="14">
+      <c r="A23" s="148">
         <f>0.0003/(2*0.025)</f>
         <v>5.9999999999999993E-3</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="122">
         <f t="shared" si="8"/>
         <v>38.888888888888893</v>
       </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="9">
+      <c r="C23" s="12"/>
+      <c r="D23" s="8">
         <v>250</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="12">
         <f t="shared" si="5"/>
         <v>70</v>
       </c>
-      <c r="G23" s="8">
+      <c r="G23" s="146">
         <f>0.0003/(2*0.025)</f>
         <v>5.9999999999999993E-3</v>
       </c>
-      <c r="H23" s="83">
+      <c r="H23" s="120">
         <f t="shared" si="9"/>
         <v>43.5</v>
       </c>
-      <c r="I23" s="10"/>
-      <c r="J23" s="9">
+      <c r="I23" s="9"/>
+      <c r="J23" s="8">
         <v>287</v>
       </c>
-      <c r="K23" s="14">
+      <c r="K23" s="12">
         <f t="shared" si="6"/>
         <v>87</v>
       </c>
-      <c r="M23" s="67">
+      <c r="M23" s="144">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="N23" s="86">
+      <c r="N23" s="117">
         <f t="shared" si="7"/>
         <v>41.194444444444443</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="15">
+      <c r="A24" s="149">
         <f>0.0003/(2*0.02)</f>
         <v>7.4999999999999989E-3</v>
       </c>
-      <c r="B24" s="12">
+      <c r="B24" s="123">
         <f t="shared" si="8"/>
         <v>42.777777777777779</v>
       </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="12">
+      <c r="C24" s="13"/>
+      <c r="D24" s="10">
         <v>257</v>
       </c>
-      <c r="E24" s="15">
+      <c r="E24" s="13">
         <f t="shared" si="5"/>
         <v>77</v>
       </c>
-      <c r="G24" s="11">
+      <c r="G24" s="147">
         <f>0.0003/(2*0.02)</f>
         <v>7.4999999999999989E-3</v>
       </c>
-      <c r="H24" s="84">
+      <c r="H24" s="121">
         <f t="shared" si="9"/>
         <v>52.5</v>
       </c>
-      <c r="I24" s="13"/>
-      <c r="J24" s="12">
+      <c r="I24" s="11"/>
+      <c r="J24" s="10">
         <v>305</v>
       </c>
-      <c r="K24" s="15">
+      <c r="K24" s="13">
         <f t="shared" si="6"/>
         <v>105</v>
       </c>
-      <c r="M24" s="68">
+      <c r="M24" s="145">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="N24" s="87">
+      <c r="N24" s="118">
         <f t="shared" si="7"/>
         <v>47.638888888888886</v>
       </c>
@@ -15137,391 +15178,391 @@
       <c r="E25" s="7"/>
       <c r="G25" s="6"/>
       <c r="K25" s="7"/>
-      <c r="M25" s="50"/>
-      <c r="N25" s="51"/>
+      <c r="M25" s="48"/>
+      <c r="N25" s="49"/>
     </row>
     <row r="26" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="107" t="s">
+      <c r="A26" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="108"/>
-      <c r="C26" s="108"/>
-      <c r="D26" s="108"/>
-      <c r="E26" s="109"/>
-      <c r="G26" s="107" t="s">
+      <c r="B26" s="104"/>
+      <c r="C26" s="104"/>
+      <c r="D26" s="104"/>
+      <c r="E26" s="105"/>
+      <c r="G26" s="103" t="s">
         <v>16</v>
       </c>
-      <c r="H26" s="108"/>
-      <c r="I26" s="108"/>
-      <c r="J26" s="108"/>
-      <c r="K26" s="109"/>
-      <c r="M26" s="123" t="s">
+      <c r="H26" s="104"/>
+      <c r="I26" s="104"/>
+      <c r="J26" s="104"/>
+      <c r="K26" s="105"/>
+      <c r="M26" s="106" t="s">
         <v>7</v>
       </c>
-      <c r="N26" s="124"/>
+      <c r="N26" s="107"/>
     </row>
     <row r="27" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="26" t="s">
+      <c r="D27" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="78" t="s">
+      <c r="E27" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="G27" s="21" t="s">
+      <c r="G27" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="H27" s="77" t="s">
+      <c r="H27" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="I27" s="22" t="s">
+      <c r="I27" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="J27" s="26" t="s">
+      <c r="J27" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="K27" s="78" t="s">
+      <c r="K27" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="M27" s="53" t="s">
+      <c r="M27" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="N27" s="73" t="s">
+      <c r="N27" s="61" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A28" s="23">
+      <c r="A28" s="150">
         <v>0</v>
       </c>
-      <c r="B28" s="27">
+      <c r="B28" s="124">
         <v>0</v>
       </c>
-      <c r="C28" s="20">
+      <c r="C28" s="18">
         <v>130</v>
       </c>
-      <c r="D28" s="23">
+      <c r="D28" s="21">
         <v>130</v>
       </c>
-      <c r="E28" s="140">
+      <c r="E28" s="76">
         <f>D28-$C$28</f>
         <v>0</v>
       </c>
-      <c r="G28" s="23">
+      <c r="G28" s="150">
         <v>0</v>
       </c>
-      <c r="H28" s="97">
+      <c r="H28" s="126">
         <v>0</v>
       </c>
-      <c r="I28" s="20">
+      <c r="I28" s="18">
         <v>70</v>
       </c>
-      <c r="J28" s="23">
+      <c r="J28" s="21">
         <v>70</v>
       </c>
-      <c r="K28" s="140">
+      <c r="K28" s="76">
         <f>J28-$I$28</f>
         <v>0</v>
       </c>
-      <c r="M28" s="54">
+      <c r="M28" s="152">
         <v>0</v>
       </c>
-      <c r="N28" s="88">
+      <c r="N28" s="129">
         <f>(B28+H28)/2</f>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A29" s="23">
+      <c r="A29" s="150">
         <f>0.0003/(2*0.05)</f>
         <v>2.9999999999999996E-3</v>
       </c>
-      <c r="B29" s="27">
+      <c r="B29" s="124">
         <f>E29/$C$28 *100</f>
         <v>5.384615384615385</v>
       </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="23">
+      <c r="C29" s="18"/>
+      <c r="D29" s="21">
         <v>137</v>
       </c>
-      <c r="E29" s="27">
+      <c r="E29" s="25">
         <f t="shared" ref="E29:E35" si="10">D29-$C$28</f>
         <v>7</v>
       </c>
-      <c r="G29" s="23">
+      <c r="G29" s="150">
         <f>0.0003/(2*0.05)</f>
         <v>2.9999999999999996E-3</v>
       </c>
-      <c r="H29" s="98">
+      <c r="H29" s="127">
         <f>K29/$I$28 *100</f>
         <v>4.2857142857142856</v>
       </c>
-      <c r="I29" s="20"/>
-      <c r="J29" s="23">
+      <c r="I29" s="18"/>
+      <c r="J29" s="21">
         <v>73</v>
       </c>
-      <c r="K29" s="27">
+      <c r="K29" s="25">
         <f t="shared" ref="K29:K35" si="11">J29-$I$28</f>
         <v>3</v>
       </c>
-      <c r="M29" s="54">
+      <c r="M29" s="152">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="N29" s="89">
+      <c r="N29" s="130">
         <f t="shared" ref="N29:N35" si="12">(B29+H29)/2</f>
         <v>4.8351648351648358</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A30" s="23">
+      <c r="A30" s="150">
         <f>0.0003/(2*0.045)</f>
         <v>3.3333333333333331E-3</v>
       </c>
-      <c r="B30" s="27">
+      <c r="B30" s="124">
         <f t="shared" ref="B30:B35" si="13">E30/$C$28 *100</f>
         <v>6.9230769230769234</v>
       </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="23">
+      <c r="C30" s="18"/>
+      <c r="D30" s="21">
         <v>139</v>
       </c>
-      <c r="E30" s="27">
+      <c r="E30" s="25">
         <f t="shared" si="10"/>
         <v>9</v>
       </c>
-      <c r="G30" s="23">
+      <c r="G30" s="150">
         <f>0.0003/(2*0.045)</f>
         <v>3.3333333333333331E-3</v>
       </c>
-      <c r="H30" s="98">
+      <c r="H30" s="127">
         <f t="shared" ref="H30:H35" si="14">K30/$I$28 *100</f>
         <v>10</v>
       </c>
-      <c r="I30" s="20"/>
-      <c r="J30" s="23">
+      <c r="I30" s="18"/>
+      <c r="J30" s="21">
         <v>77</v>
       </c>
-      <c r="K30" s="27">
+      <c r="K30" s="25">
         <f t="shared" si="11"/>
         <v>7</v>
       </c>
-      <c r="M30" s="54">
+      <c r="M30" s="152">
         <v>3.333333E-3</v>
       </c>
-      <c r="N30" s="89">
+      <c r="N30" s="130">
         <f t="shared" si="12"/>
         <v>8.4615384615384617</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A31" s="23">
+      <c r="A31" s="150">
         <f>0.0003/(2*0.04)</f>
         <v>3.7499999999999994E-3</v>
       </c>
-      <c r="B31" s="27">
+      <c r="B31" s="124">
         <f t="shared" si="13"/>
         <v>9.2307692307692317</v>
       </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="23">
+      <c r="C31" s="18"/>
+      <c r="D31" s="21">
         <v>142</v>
       </c>
-      <c r="E31" s="27">
+      <c r="E31" s="25">
         <f t="shared" si="10"/>
         <v>12</v>
       </c>
-      <c r="G31" s="23">
+      <c r="G31" s="150">
         <f>0.0003/(2*0.04)</f>
         <v>3.7499999999999994E-3</v>
       </c>
-      <c r="H31" s="98">
+      <c r="H31" s="127">
         <f t="shared" si="14"/>
         <v>11.428571428571429</v>
       </c>
-      <c r="I31" s="20"/>
-      <c r="J31" s="23">
+      <c r="I31" s="18"/>
+      <c r="J31" s="21">
         <v>78</v>
       </c>
-      <c r="K31" s="27">
+      <c r="K31" s="25">
         <f t="shared" si="11"/>
         <v>8</v>
       </c>
-      <c r="M31" s="54">
+      <c r="M31" s="152">
         <v>3.7499999999999999E-3</v>
       </c>
-      <c r="N31" s="89">
+      <c r="N31" s="130">
         <f t="shared" si="12"/>
         <v>10.32967032967033</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A32" s="23">
+      <c r="A32" s="150">
         <f>0.0003/(2*0.035)</f>
         <v>4.2857142857142851E-3</v>
       </c>
-      <c r="B32" s="27">
+      <c r="B32" s="124">
         <f t="shared" si="13"/>
         <v>15.384615384615385</v>
       </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="23">
+      <c r="C32" s="18"/>
+      <c r="D32" s="21">
         <v>150</v>
       </c>
-      <c r="E32" s="27">
+      <c r="E32" s="25">
         <f t="shared" si="10"/>
         <v>20</v>
       </c>
-      <c r="G32" s="23">
+      <c r="G32" s="150">
         <f>0.0003/(2*0.035)</f>
         <v>4.2857142857142851E-3</v>
       </c>
-      <c r="H32" s="98">
+      <c r="H32" s="127">
         <f t="shared" si="14"/>
         <v>17.142857142857142</v>
       </c>
-      <c r="I32" s="20"/>
-      <c r="J32" s="23">
+      <c r="I32" s="18"/>
+      <c r="J32" s="21">
         <v>82</v>
       </c>
-      <c r="K32" s="27">
+      <c r="K32" s="25">
         <f t="shared" si="11"/>
         <v>12</v>
       </c>
-      <c r="M32" s="54">
+      <c r="M32" s="152">
         <v>4.2857140000000004E-3</v>
       </c>
-      <c r="N32" s="89">
+      <c r="N32" s="130">
         <f t="shared" si="12"/>
         <v>16.263736263736263</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A33" s="23">
+      <c r="A33" s="150">
         <f>0.0003/(2*0.03)</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="B33" s="27">
+      <c r="B33" s="124">
         <f t="shared" si="13"/>
         <v>16.923076923076923</v>
       </c>
-      <c r="C33" s="20"/>
-      <c r="D33" s="23">
+      <c r="C33" s="18"/>
+      <c r="D33" s="21">
         <v>152</v>
       </c>
-      <c r="E33" s="27">
+      <c r="E33" s="25">
         <f t="shared" si="10"/>
         <v>22</v>
       </c>
-      <c r="G33" s="23">
+      <c r="G33" s="150">
         <f>0.0003/(2*0.03)</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H33" s="98">
+      <c r="H33" s="127">
         <f t="shared" si="14"/>
         <v>4.2857142857142856</v>
       </c>
-      <c r="I33" s="20"/>
-      <c r="J33" s="23">
+      <c r="I33" s="18"/>
+      <c r="J33" s="21">
         <v>73</v>
       </c>
-      <c r="K33" s="27">
+      <c r="K33" s="25">
         <f t="shared" si="11"/>
         <v>3</v>
       </c>
-      <c r="M33" s="54">
+      <c r="M33" s="152">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="N33" s="89">
+      <c r="N33" s="130">
         <f t="shared" si="12"/>
         <v>10.604395604395604</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A34" s="23">
+      <c r="A34" s="150">
         <f>0.0003/(2*0.025)</f>
         <v>5.9999999999999993E-3</v>
       </c>
-      <c r="B34" s="27">
+      <c r="B34" s="124">
         <f t="shared" si="13"/>
         <v>23.846153846153847</v>
       </c>
-      <c r="C34" s="20"/>
-      <c r="D34" s="23">
+      <c r="C34" s="18"/>
+      <c r="D34" s="21">
         <v>161</v>
       </c>
-      <c r="E34" s="27">
+      <c r="E34" s="25">
         <f t="shared" si="10"/>
         <v>31</v>
       </c>
-      <c r="G34" s="23">
+      <c r="G34" s="150">
         <f>0.0003/(2*0.025)</f>
         <v>5.9999999999999993E-3</v>
       </c>
-      <c r="H34" s="98">
+      <c r="H34" s="127">
         <f t="shared" si="14"/>
         <v>18.571428571428573</v>
       </c>
-      <c r="I34" s="20"/>
-      <c r="J34" s="23">
+      <c r="I34" s="18"/>
+      <c r="J34" s="21">
         <v>83</v>
       </c>
-      <c r="K34" s="27">
+      <c r="K34" s="25">
         <f t="shared" si="11"/>
         <v>13</v>
       </c>
-      <c r="M34" s="54">
+      <c r="M34" s="152">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="N34" s="89">
+      <c r="N34" s="130">
         <f t="shared" si="12"/>
         <v>21.208791208791212</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="24">
+      <c r="A35" s="151">
         <f>0.0003/(2*0.02)</f>
         <v>7.4999999999999989E-3</v>
       </c>
-      <c r="B35" s="28">
+      <c r="B35" s="125">
         <f t="shared" si="13"/>
         <v>30.76923076923077</v>
       </c>
-      <c r="C35" s="25"/>
-      <c r="D35" s="24">
+      <c r="C35" s="23"/>
+      <c r="D35" s="22">
         <v>170</v>
       </c>
-      <c r="E35" s="28">
+      <c r="E35" s="26">
         <f t="shared" si="10"/>
         <v>40</v>
       </c>
-      <c r="G35" s="24">
+      <c r="G35" s="151">
         <f>0.0003/(2*0.02)</f>
         <v>7.4999999999999989E-3</v>
       </c>
-      <c r="H35" s="99">
+      <c r="H35" s="128">
         <f t="shared" si="14"/>
         <v>28.571428571428569</v>
       </c>
-      <c r="I35" s="25"/>
-      <c r="J35" s="24">
+      <c r="I35" s="23"/>
+      <c r="J35" s="22">
         <v>90</v>
       </c>
-      <c r="K35" s="28">
+      <c r="K35" s="26">
         <f t="shared" si="11"/>
         <v>20</v>
       </c>
-      <c r="M35" s="55">
+      <c r="M35" s="153">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="N35" s="90">
+      <c r="N35" s="131">
         <f t="shared" si="12"/>
         <v>29.670329670329672</v>
       </c>
@@ -15531,391 +15572,391 @@
       <c r="E36" s="7"/>
       <c r="G36" s="6"/>
       <c r="K36" s="7"/>
-      <c r="M36" s="50"/>
-      <c r="N36" s="51"/>
+      <c r="M36" s="48"/>
+      <c r="N36" s="49"/>
     </row>
     <row r="37" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="110" t="s">
+      <c r="A37" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="111"/>
-      <c r="C37" s="111"/>
-      <c r="D37" s="111"/>
-      <c r="E37" s="112"/>
-      <c r="G37" s="110" t="s">
+      <c r="B37" s="94"/>
+      <c r="C37" s="94"/>
+      <c r="D37" s="94"/>
+      <c r="E37" s="95"/>
+      <c r="G37" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="H37" s="111"/>
-      <c r="I37" s="111"/>
-      <c r="J37" s="111"/>
-      <c r="K37" s="112"/>
-      <c r="M37" s="125" t="s">
+      <c r="H37" s="94"/>
+      <c r="I37" s="94"/>
+      <c r="J37" s="94"/>
+      <c r="K37" s="95"/>
+      <c r="M37" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="N37" s="126"/>
+      <c r="N37" s="97"/>
     </row>
     <row r="38" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="30" t="s">
+      <c r="A38" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="33" t="s">
+      <c r="B38" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="31" t="s">
+      <c r="C38" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="D38" s="33" t="s">
+      <c r="D38" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E38" s="75" t="s">
+      <c r="E38" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="G38" s="30" t="s">
+      <c r="G38" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="H38" s="76" t="s">
+      <c r="H38" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="I38" s="31" t="s">
+      <c r="I38" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="J38" s="33" t="s">
+      <c r="J38" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="K38" s="75" t="s">
+      <c r="K38" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="M38" s="56" t="s">
+      <c r="M38" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="N38" s="74" t="s">
+      <c r="N38" s="62" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A39" s="36">
+      <c r="A39" s="156">
         <v>0</v>
       </c>
-      <c r="B39" s="34">
+      <c r="B39" s="132">
         <v>0</v>
       </c>
-      <c r="C39" s="29">
+      <c r="C39" s="27">
         <v>100</v>
       </c>
-      <c r="D39" s="36">
+      <c r="D39" s="34">
         <v>100</v>
       </c>
-      <c r="E39" s="133">
+      <c r="E39" s="69">
         <f>D39-$C$39</f>
         <v>0</v>
       </c>
-      <c r="G39" s="36">
+      <c r="G39" s="156">
         <v>0</v>
       </c>
-      <c r="H39" s="94">
+      <c r="H39" s="134">
         <v>0</v>
       </c>
-      <c r="I39" s="29">
+      <c r="I39" s="27">
         <v>102</v>
       </c>
-      <c r="J39" s="36">
+      <c r="J39" s="34">
         <v>102</v>
       </c>
-      <c r="K39" s="133">
+      <c r="K39" s="69">
         <f>J39-$I$39</f>
         <v>0</v>
       </c>
-      <c r="M39" s="57">
+      <c r="M39" s="154">
         <v>0</v>
       </c>
-      <c r="N39" s="91">
+      <c r="N39" s="137">
         <f>(B39+H39)/2</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A40" s="36">
+      <c r="A40" s="156">
         <f>0.0003/(2*0.05)</f>
         <v>2.9999999999999996E-3</v>
       </c>
-      <c r="B40" s="34">
+      <c r="B40" s="132">
         <f>E40/$C$39 *100</f>
         <v>17</v>
       </c>
-      <c r="C40" s="29"/>
-      <c r="D40" s="36">
+      <c r="C40" s="27"/>
+      <c r="D40" s="34">
         <v>117</v>
       </c>
-      <c r="E40" s="34">
+      <c r="E40" s="32">
         <f t="shared" ref="E40:E46" si="15">D40-$C$39</f>
         <v>17</v>
       </c>
-      <c r="G40" s="36">
+      <c r="G40" s="156">
         <f>0.0003/(2*0.05)</f>
         <v>2.9999999999999996E-3</v>
       </c>
-      <c r="H40" s="95">
+      <c r="H40" s="135">
         <f>K40/$I$39 *100</f>
         <v>0.98039215686274506</v>
       </c>
-      <c r="I40" s="29"/>
-      <c r="J40" s="36">
+      <c r="I40" s="27"/>
+      <c r="J40" s="34">
         <v>103</v>
       </c>
-      <c r="K40" s="34">
+      <c r="K40" s="32">
         <f t="shared" ref="K40:K46" si="16">J40-$I$39</f>
         <v>1</v>
       </c>
-      <c r="M40" s="57">
+      <c r="M40" s="154">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="N40" s="92">
+      <c r="N40" s="138">
         <f t="shared" ref="N40:N46" si="17">(B40+H40)/2</f>
         <v>8.9901960784313726</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A41" s="36">
+      <c r="A41" s="156">
         <f>0.0003/(2*0.045)</f>
         <v>3.3333333333333331E-3</v>
       </c>
-      <c r="B41" s="34">
+      <c r="B41" s="132">
         <f t="shared" ref="B41:B46" si="18">E41/$C$39 *100</f>
         <v>20</v>
       </c>
-      <c r="C41" s="29"/>
-      <c r="D41" s="36">
+      <c r="C41" s="27"/>
+      <c r="D41" s="34">
         <v>120</v>
       </c>
-      <c r="E41" s="34">
+      <c r="E41" s="32">
         <f t="shared" si="15"/>
         <v>20</v>
       </c>
-      <c r="G41" s="36">
+      <c r="G41" s="156">
         <f>0.0003/(2*0.045)</f>
         <v>3.3333333333333331E-3</v>
       </c>
-      <c r="H41" s="95">
+      <c r="H41" s="135">
         <f t="shared" ref="H41:H46" si="19">K41/$I$39 *100</f>
         <v>4.9019607843137258</v>
       </c>
-      <c r="I41" s="29"/>
-      <c r="J41" s="36">
+      <c r="I41" s="27"/>
+      <c r="J41" s="34">
         <v>107</v>
       </c>
-      <c r="K41" s="34">
+      <c r="K41" s="32">
         <f t="shared" si="16"/>
         <v>5</v>
       </c>
-      <c r="M41" s="57">
+      <c r="M41" s="154">
         <v>3.333333E-3</v>
       </c>
-      <c r="N41" s="92">
+      <c r="N41" s="138">
         <f t="shared" si="17"/>
         <v>12.450980392156863</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A42" s="36">
+      <c r="A42" s="156">
         <f>0.0003/(2*0.04)</f>
         <v>3.7499999999999994E-3</v>
       </c>
-      <c r="B42" s="34">
+      <c r="B42" s="132">
         <f t="shared" si="18"/>
         <v>26</v>
       </c>
-      <c r="C42" s="29"/>
-      <c r="D42" s="36">
+      <c r="C42" s="27"/>
+      <c r="D42" s="34">
         <v>126</v>
       </c>
-      <c r="E42" s="34">
+      <c r="E42" s="32">
         <f t="shared" si="15"/>
         <v>26</v>
       </c>
-      <c r="G42" s="36">
+      <c r="G42" s="156">
         <f>0.0003/(2*0.04)</f>
         <v>3.7499999999999994E-3</v>
       </c>
-      <c r="H42" s="95">
+      <c r="H42" s="135">
         <f t="shared" si="19"/>
         <v>13.725490196078432</v>
       </c>
-      <c r="I42" s="29"/>
-      <c r="J42" s="36">
+      <c r="I42" s="27"/>
+      <c r="J42" s="34">
         <v>116</v>
       </c>
-      <c r="K42" s="34">
+      <c r="K42" s="32">
         <f t="shared" si="16"/>
         <v>14</v>
       </c>
-      <c r="M42" s="57">
+      <c r="M42" s="154">
         <v>3.7499999999999999E-3</v>
       </c>
-      <c r="N42" s="92">
+      <c r="N42" s="138">
         <f t="shared" si="17"/>
         <v>19.862745098039216</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A43" s="36">
+      <c r="A43" s="156">
         <f>0.0003/(2*0.035)</f>
         <v>4.2857142857142851E-3</v>
       </c>
-      <c r="B43" s="34">
+      <c r="B43" s="132">
         <f t="shared" si="18"/>
         <v>31</v>
       </c>
-      <c r="C43" s="29"/>
-      <c r="D43" s="36">
+      <c r="C43" s="27"/>
+      <c r="D43" s="34">
         <v>131</v>
       </c>
-      <c r="E43" s="34">
+      <c r="E43" s="32">
         <f t="shared" si="15"/>
         <v>31</v>
       </c>
-      <c r="G43" s="36">
+      <c r="G43" s="156">
         <f>0.0003/(2*0.035)</f>
         <v>4.2857142857142851E-3</v>
       </c>
-      <c r="H43" s="95">
+      <c r="H43" s="135">
         <f t="shared" si="19"/>
         <v>20.588235294117645</v>
       </c>
-      <c r="I43" s="29"/>
-      <c r="J43" s="36">
+      <c r="I43" s="27"/>
+      <c r="J43" s="34">
         <v>123</v>
       </c>
-      <c r="K43" s="34">
+      <c r="K43" s="32">
         <f t="shared" si="16"/>
         <v>21</v>
       </c>
-      <c r="M43" s="57">
+      <c r="M43" s="154">
         <v>4.2857140000000004E-3</v>
       </c>
-      <c r="N43" s="92">
+      <c r="N43" s="138">
         <f t="shared" si="17"/>
         <v>25.794117647058822</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A44" s="36">
+      <c r="A44" s="156">
         <f>0.0003/(2*0.03)</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="B44" s="34">
+      <c r="B44" s="132">
         <f t="shared" si="18"/>
         <v>28.999999999999996</v>
       </c>
-      <c r="C44" s="29"/>
-      <c r="D44" s="36">
+      <c r="C44" s="27"/>
+      <c r="D44" s="34">
         <v>129</v>
       </c>
-      <c r="E44" s="34">
+      <c r="E44" s="32">
         <f t="shared" si="15"/>
         <v>29</v>
       </c>
-      <c r="G44" s="36">
+      <c r="G44" s="156">
         <f>0.0003/(2*0.03)</f>
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H44" s="95">
+      <c r="H44" s="135">
         <f t="shared" si="19"/>
         <v>22.549019607843139</v>
       </c>
-      <c r="I44" s="29"/>
-      <c r="J44" s="36">
+      <c r="I44" s="27"/>
+      <c r="J44" s="34">
         <v>125</v>
       </c>
-      <c r="K44" s="34">
+      <c r="K44" s="32">
         <f t="shared" si="16"/>
         <v>23</v>
       </c>
-      <c r="M44" s="57">
+      <c r="M44" s="154">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="N44" s="92">
+      <c r="N44" s="138">
         <f t="shared" si="17"/>
         <v>25.774509803921568</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A45" s="36">
+      <c r="A45" s="156">
         <f>0.0003/(2*0.025)</f>
         <v>5.9999999999999993E-3</v>
       </c>
-      <c r="B45" s="34">
+      <c r="B45" s="132">
         <f t="shared" si="18"/>
         <v>34</v>
       </c>
-      <c r="C45" s="29"/>
-      <c r="D45" s="36">
+      <c r="C45" s="27"/>
+      <c r="D45" s="34">
         <v>134</v>
       </c>
-      <c r="E45" s="34">
+      <c r="E45" s="32">
         <f t="shared" si="15"/>
         <v>34</v>
       </c>
-      <c r="G45" s="36">
+      <c r="G45" s="156">
         <f>0.0003/(2*0.025)</f>
         <v>5.9999999999999993E-3</v>
       </c>
-      <c r="H45" s="95">
+      <c r="H45" s="135">
         <f t="shared" si="19"/>
         <v>27.450980392156865</v>
       </c>
-      <c r="I45" s="29"/>
-      <c r="J45" s="36">
+      <c r="I45" s="27"/>
+      <c r="J45" s="34">
         <v>130</v>
       </c>
-      <c r="K45" s="34">
+      <c r="K45" s="32">
         <f t="shared" si="16"/>
         <v>28</v>
       </c>
-      <c r="M45" s="57">
+      <c r="M45" s="154">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="N45" s="92">
+      <c r="N45" s="138">
         <f t="shared" si="17"/>
         <v>30.725490196078432</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="38">
+      <c r="A46" s="157">
         <f>0.0003/(2*0.02)</f>
         <v>7.4999999999999989E-3</v>
       </c>
-      <c r="B46" s="35">
+      <c r="B46" s="133">
         <f t="shared" si="18"/>
         <v>40</v>
       </c>
-      <c r="C46" s="39"/>
-      <c r="D46" s="38">
+      <c r="C46" s="37"/>
+      <c r="D46" s="36">
         <v>140</v>
       </c>
-      <c r="E46" s="35">
+      <c r="E46" s="33">
         <f t="shared" si="15"/>
         <v>40</v>
       </c>
-      <c r="G46" s="38">
+      <c r="G46" s="157">
         <f>0.0003/(2*0.02)</f>
         <v>7.4999999999999989E-3</v>
       </c>
-      <c r="H46" s="96">
+      <c r="H46" s="136">
         <f t="shared" si="19"/>
         <v>34.313725490196077</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="38">
+      <c r="I46" s="37"/>
+      <c r="J46" s="36">
         <v>137</v>
       </c>
-      <c r="K46" s="35">
+      <c r="K46" s="33">
         <f t="shared" si="16"/>
         <v>35</v>
       </c>
-      <c r="M46" s="58">
+      <c r="M46" s="155">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="N46" s="93">
+      <c r="N46" s="139">
         <f t="shared" si="17"/>
         <v>37.156862745098039</v>
       </c>

</xml_diff>